<commit_message>
Correct formatting of BR2 workbook
</commit_message>
<xml_diff>
--- a/tests/bin/sample_BR2_reports.xlsx
+++ b/tests/bin/sample_BR2_reports.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC7CD21-4096-43AA-86F3-7349739D5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="57480" yWindow="-7740" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EBSCO 16-17" sheetId="1" r:id="rId1"/>
     <sheet name="PQ 16-17" sheetId="3" r:id="rId2"/>
-    <sheet name="Gale 16-17" sheetId="15" r:id="rId3"/>
+    <sheet name="Gale 16-17" sheetId="16" r:id="rId3"/>
     <sheet name="EBSCO 17-18" sheetId="4" r:id="rId4"/>
     <sheet name="PQ 17-18" sheetId="6" r:id="rId5"/>
     <sheet name="Gale 17-18" sheetId="12" r:id="rId6"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="107">
   <si>
     <t/>
   </si>
@@ -363,7 +364,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,16 +715,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -731,7 +732,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -739,7 +740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -747,27 +748,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -826,7 +827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -849,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -908,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -967,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1027,8 +1028,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:T8">
-    <sortState ref="A9:U12">
+  <autoFilter ref="A8:T8" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:U12">
       <sortCondition sortBy="cellColor" ref="A8" dxfId="2"/>
     </sortState>
   </autoFilter>
@@ -1037,16 +1038,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>4840</v>
       </c>
@@ -1070,27 +1071,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="4">
         <v>43075</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1149,12 +1150,12 @@
         <v>42887</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1207,26 +1208,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF58698E-1036-4F90-AABB-80F95548750F}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1248,64 +1239,49 @@
       <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I1" s="3">
+        <v>42552</v>
+      </c>
+      <c r="J1" s="3">
+        <v>42583</v>
+      </c>
+      <c r="K1" s="3">
+        <v>42614</v>
+      </c>
+      <c r="L1" s="3">
+        <v>42644</v>
+      </c>
+      <c r="M1" s="3">
+        <v>42675</v>
+      </c>
+      <c r="N1" s="3">
+        <v>42705</v>
+      </c>
+      <c r="O1" s="3">
+        <v>42736</v>
+      </c>
+      <c r="P1" s="3">
+        <v>42767</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>42795</v>
+      </c>
+      <c r="R1" s="3">
+        <v>42826</v>
+      </c>
+      <c r="S1" s="3">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1315,9 +1291,6 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
       <c r="E3" t="s">
         <v>57</v>
       </c>
@@ -1358,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1368,9 +1341,6 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
       <c r="E4" t="s">
         <v>57</v>
       </c>
@@ -1411,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1421,9 +1391,6 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
       <c r="E5" t="s">
         <v>57</v>
       </c>
@@ -1467,7 +1434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1477,9 +1444,6 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
       <c r="E6" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1533,9 +1497,6 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
       <c r="E7" t="s">
         <v>51</v>
       </c>
@@ -1573,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1583,9 +1544,6 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
       <c r="E8" t="s">
         <v>51</v>
       </c>
@@ -1626,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1636,9 +1594,6 @@
       <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
       <c r="E9" t="s">
         <v>51</v>
       </c>
@@ -1679,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1689,9 +1644,6 @@
       <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
       <c r="E10" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1742,9 +1694,6 @@
       <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
@@ -1785,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1795,9 +1744,6 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
       <c r="E12" t="s">
         <v>35</v>
       </c>
@@ -1838,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1848,9 +1794,6 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
-        <v>0</v>
-      </c>
       <c r="E13" t="s">
         <v>35</v>
       </c>
@@ -1894,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1904,9 +1847,6 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
-        <v>0</v>
-      </c>
       <c r="E14" t="s">
         <v>35</v>
       </c>
@@ -1950,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1960,9 +1900,6 @@
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
@@ -2002,20 +1939,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -2023,7 +1961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -2031,32 +1969,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2115,7 +2053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2138,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2194,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2253,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2309,7 +2247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2366,8 +2304,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:T8">
-    <sortState ref="A9:U13">
+  <autoFilter ref="A8:T8" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:U13">
       <sortCondition sortBy="cellColor" ref="A8" dxfId="1"/>
     </sortState>
   </autoFilter>
@@ -2376,16 +2314,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -2393,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2401,7 +2339,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>4840</v>
       </c>
@@ -2409,27 +2347,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="4">
         <v>43308</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -2488,12 +2426,12 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2540,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -2596,19 +2534,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -2667,7 +2605,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2690,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2749,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2808,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2864,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2920,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2976,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -3035,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -3094,16 +3032,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -3111,7 +3049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>105</v>
       </c>
@@ -3119,32 +3057,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3203,7 +3141,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3226,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3282,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3339,8 +3277,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:T8">
-    <sortState ref="A9:U11">
+  <autoFilter ref="A8:T8" xr:uid="{00000000-0009-0000-0000-000006000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:U11">
       <sortCondition sortBy="cellColor" ref="A8" dxfId="0"/>
     </sortState>
   </autoFilter>
@@ -3349,16 +3287,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3366,7 +3304,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3374,7 +3312,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>4840</v>
       </c>
@@ -3382,27 +3320,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" s="4">
         <v>43692</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -3461,12 +3399,12 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -3519,16 +3457,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>106</v>
       </c>
@@ -3590,7 +3528,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3613,7 +3551,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3672,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3728,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3784,7 +3722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -3840,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3896,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>38</v>
       </c>

</xml_diff>